<commit_message>
Updating UWP compatibility info
</commit_message>
<xml_diff>
--- a/compatibility.xlsx
+++ b/compatibility.xlsx
@@ -2342,9 +2342,6 @@
     <t>test\simple\test-zlib-convenience-methods.js</t>
   </si>
   <si>
-    <t>Yes *stdout/stderr is redirected to file*</t>
-  </si>
-  <si>
     <t>UWP Support (Yes/No)</t>
   </si>
   <si>
@@ -2388,6 +2385,9 @@
   </si>
   <si>
     <t>ZLIB</t>
+  </si>
+  <si>
+    <t>No (output can optionally be redirected to file)</t>
   </si>
 </sst>
 </file>
@@ -2887,14 +2887,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E850"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B812" sqref="B812"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
@@ -2902,16 +2902,16 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>13</v>
@@ -3699,7 +3699,7 @@
     </row>
     <row r="78" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="42" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B78" s="31" t="s">
         <v>76</v>
@@ -3735,8 +3735,8 @@
       <c r="A84" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B84" s="23" t="s">
-        <v>772</v>
+      <c r="B84" s="15" t="s">
+        <v>787</v>
       </c>
       <c r="C84" s="37" t="s">
         <v>191</v>
@@ -5893,7 +5893,7 @@
     </row>
     <row r="450" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A450" s="24" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B450" s="23" t="s">
         <v>63</v>
@@ -6239,7 +6239,7 @@
     </row>
     <row r="511" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A511" s="24" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B511" s="23" t="s">
         <v>63</v>
@@ -6521,7 +6521,7 @@
     </row>
     <row r="545" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A545" s="24" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B545" s="23" t="s">
         <v>63</v>
@@ -6743,7 +6743,7 @@
     </row>
     <row r="586" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A586" s="24" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B586" s="23" t="s">
         <v>63</v>
@@ -6821,7 +6821,7 @@
     </row>
     <row r="597" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A597" s="24" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B597" s="23" t="s">
         <v>63</v>
@@ -7323,7 +7323,7 @@
     </row>
     <row r="681" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A681" s="24" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B681" s="23" t="s">
         <v>63</v>
@@ -7732,7 +7732,7 @@
     </row>
     <row r="750" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A750" s="24" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B750" s="23" t="s">
         <v>63</v>
@@ -7947,7 +7947,7 @@
     </row>
     <row r="779" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A779" s="24" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B779" s="23" t="s">
         <v>63</v>
@@ -8058,7 +8058,7 @@
     </row>
     <row r="799" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A799" s="24" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B799" s="23" t="s">
         <v>63</v>
@@ -8157,7 +8157,7 @@
     </row>
     <row r="813" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A813" s="24" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B813" s="23" t="s">
         <v>63</v>

</xml_diff>